<commit_message>
Additive Results++: 200 epochs and LR 0.0001
</commit_message>
<xml_diff>
--- a/yield_prediction/results/graph_descriptors/WL_gnn/out_of_sample/additive/ranking_test2/results.xlsx
+++ b/yield_prediction/results/graph_descriptors/WL_gnn/out_of_sample/additive/ranking_test2/results.xlsx
@@ -412,7 +412,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K90"/>
+  <dimension ref="A1:K96"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:B19"/>
@@ -4304,6 +4304,264 @@
         <v>18.282</v>
       </c>
     </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>additive_200epochs</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>ranking_test2</t>
+        </is>
+      </c>
+      <c r="C91" t="n">
+        <v>3</v>
+      </c>
+      <c r="D91" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>mean</t>
+        </is>
+      </c>
+      <c r="F91" t="inlineStr">
+        <is>
+          <t>product</t>
+        </is>
+      </c>
+      <c r="G91" t="n">
+        <v>198.448</v>
+      </c>
+      <c r="H91" t="n">
+        <v>0.767</v>
+      </c>
+      <c r="I91" t="n">
+        <v>12.781</v>
+      </c>
+      <c r="J91" t="n">
+        <v>0.237</v>
+      </c>
+      <c r="K91" t="n">
+        <v>17.706</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>additive_200epochs</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>ranking_test2</t>
+        </is>
+      </c>
+      <c r="C92" t="n">
+        <v>3</v>
+      </c>
+      <c r="D92" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>mean</t>
+        </is>
+      </c>
+      <c r="F92" t="inlineStr">
+        <is>
+          <t>product</t>
+        </is>
+      </c>
+      <c r="G92" t="n">
+        <v>287.345</v>
+      </c>
+      <c r="H92" t="n">
+        <v>0.613</v>
+      </c>
+      <c r="I92" t="n">
+        <v>16.588</v>
+      </c>
+      <c r="J92" t="n">
+        <v>0.175</v>
+      </c>
+      <c r="K92" t="n">
+        <v>19.482</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>additive_200epochs</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>ranking_test2</t>
+        </is>
+      </c>
+      <c r="C93" t="n">
+        <v>5</v>
+      </c>
+      <c r="D93" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>mean</t>
+        </is>
+      </c>
+      <c r="F93" t="inlineStr">
+        <is>
+          <t>product</t>
+        </is>
+      </c>
+      <c r="G93" t="n">
+        <v>167.498</v>
+      </c>
+      <c r="H93" t="n">
+        <v>0.773</v>
+      </c>
+      <c r="I93" t="n">
+        <v>12.605</v>
+      </c>
+      <c r="J93" t="n">
+        <v>0.337</v>
+      </c>
+      <c r="K93" t="n">
+        <v>17.072</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>additive_200epochs</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>ranking_test2</t>
+        </is>
+      </c>
+      <c r="C94" t="n">
+        <v>2</v>
+      </c>
+      <c r="D94" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>sum</t>
+        </is>
+      </c>
+      <c r="F94" t="inlineStr">
+        <is>
+          <t>product</t>
+        </is>
+      </c>
+      <c r="G94" t="n">
+        <v>281.699</v>
+      </c>
+      <c r="H94" t="n">
+        <v>0.619</v>
+      </c>
+      <c r="I94" t="n">
+        <v>16.462</v>
+      </c>
+      <c r="J94" t="n">
+        <v>0.248</v>
+      </c>
+      <c r="K94" t="n">
+        <v>18.322</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>additive_200epochs</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>ranking_test2</t>
+        </is>
+      </c>
+      <c r="C95" t="n">
+        <v>3</v>
+      </c>
+      <c r="D95" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>max</t>
+        </is>
+      </c>
+      <c r="F95" t="inlineStr">
+        <is>
+          <t>mean</t>
+        </is>
+      </c>
+      <c r="G95" t="n">
+        <v>223.099</v>
+      </c>
+      <c r="H95" t="n">
+        <v>0.712</v>
+      </c>
+      <c r="I95" t="n">
+        <v>14.326</v>
+      </c>
+      <c r="J95" t="n">
+        <v>0.273</v>
+      </c>
+      <c r="K95" t="n">
+        <v>17.479</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>additive_200epochs</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>ranking_test2</t>
+        </is>
+      </c>
+      <c r="C96" t="n">
+        <v>3</v>
+      </c>
+      <c r="D96" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>max</t>
+        </is>
+      </c>
+      <c r="F96" t="inlineStr">
+        <is>
+          <t>mean</t>
+        </is>
+      </c>
+      <c r="G96" t="n">
+        <v>355.712</v>
+      </c>
+      <c r="H96" t="n">
+        <v>0.507</v>
+      </c>
+      <c r="I96" t="n">
+        <v>18.72</v>
+      </c>
+      <c r="J96" t="n">
+        <v>0.187</v>
+      </c>
+      <c r="K96" t="n">
+        <v>19.182</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>